<commit_message>
First draft of cloud services and started comparison
</commit_message>
<xml_diff>
--- a/Fremdriftsplan.xlsx
+++ b/Fremdriftsplan.xlsx
@@ -83,10 +83,10 @@
     <t>Oppstart og få oversikt over skyløsninger</t>
   </si>
   <si>
-    <t>Vurdere kriterier for de ulike skytjenestene</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ferdigstilling av rapport </t>
+  </si>
+  <si>
+    <t>Lese om og sammenligne skytjenester</t>
   </si>
 </sst>
 </file>
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +462,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -470,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -478,7 +478,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -542,7 +542,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -558,7 +558,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -566,7 +566,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -574,7 +574,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>